<commit_message>
working on data provider util
</commit_message>
<xml_diff>
--- a/target/classes/com/testdata/RegistrationTestdata.xlsx
+++ b/target/classes/com/testdata/RegistrationTestdata.xlsx
@@ -20,7 +20,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+  <si>
+    <t xml:space="preserve">loginname</t>
+  </si>
   <si>
     <t xml:space="preserve">firstname</t>
   </si>
@@ -34,6 +37,12 @@
     <t xml:space="preserve">password</t>
   </si>
   <si>
+    <t xml:space="preserve">country</t>
+  </si>
+  <si>
+    <t xml:space="preserve">romeo@yahoo.com</t>
+  </si>
+  <si>
     <t xml:space="preserve">Romeo</t>
   </si>
   <si>
@@ -43,7 +52,13 @@
     <t xml:space="preserve">shakespeare@gmail.com</t>
   </si>
   <si>
-    <t xml:space="preserve">younglove</t>
+    <t xml:space="preserve">Younglove</t>
+  </si>
+  <si>
+    <t xml:space="preserve">United Kingdom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">creapypainting@gmail.com</t>
   </si>
   <si>
     <t xml:space="preserve">Dorian</t>
@@ -52,10 +67,13 @@
     <t xml:space="preserve">Gray</t>
   </si>
   <si>
-    <t xml:space="preserve">creapypainting@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">foreveryoung</t>
+    <t xml:space="preserve">Foreveryoung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ireland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">goodness@gmail.com</t>
   </si>
   <si>
     <t xml:space="preserve">Alesha</t>
@@ -64,10 +82,10 @@
     <t xml:space="preserve">Karamazov</t>
   </si>
   <si>
-    <t xml:space="preserve">goodness@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">drama</t>
+    <t xml:space="preserve">WarWorld</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Russia</t>
   </si>
 </sst>
 </file>
@@ -77,7 +95,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -105,6 +123,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -149,7 +172,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -159,6 +182,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -179,13 +206,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -200,54 +227,81 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
+      <c r="A2" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="1" t="s">
         <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>8</v>
+      <c r="A3" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>12</v>
+      <c r="A4" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="shakespeare@gmail.com"/>
-    <hyperlink ref="C3" r:id="rId2" display="creapypainting@gmail.com"/>
-    <hyperlink ref="C4" r:id="rId3" display="goodness@gmail.com"/>
+    <hyperlink ref="A2" r:id="rId1" display="romeo@yahoo.com"/>
+    <hyperlink ref="D2" r:id="rId2" display="shakespeare@gmail.com"/>
+    <hyperlink ref="A3" r:id="rId3" display="creapypainting@gmail.com"/>
+    <hyperlink ref="D3" r:id="rId4" display="creapypainting@gmail.com"/>
+    <hyperlink ref="A4" r:id="rId5" display="goodness@gmail.com"/>
+    <hyperlink ref="D4" r:id="rId6" display="goodness@gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>